<commit_message>
udate API handling in FE, BE config, and data
</commit_message>
<xml_diff>
--- a/camera-shop/src/main/resources/data.xlsx
+++ b/camera-shop/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\camera-shop\camera-shop\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D22DA5-BD33-458F-98E7-ADB122A46875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD03E976-967F-481D-8BD3-F74605A38F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{90887BD4-D8A2-4FD5-939A-5967D6FE0B64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{90887BD4-D8A2-4FD5-939A-5967D6FE0B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Brand" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Feature" sheetId="4" r:id="rId3"/>
     <sheet name="Camera" sheetId="5" r:id="rId4"/>
     <sheet name="Variant" sheetId="6" r:id="rId5"/>
+    <sheet name="Post" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="140">
   <si>
     <t>id</t>
   </si>
@@ -400,13 +401,106 @@
   </si>
   <si>
     <t>https://cdn.builder.io/api/v1/image/assets/TEMP/66c23dacb996a6fd02c53c8a4b9a61e456290258b8d99f22d8c84bffc4768d7f?apiKey=53e4b1c7e8314bb0af1a0d344422a86a&amp;</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>authorName</t>
+  </si>
+  <si>
+    <t>publishedAt</t>
+  </si>
+  <si>
+    <t>Fujifilm makes niche cameras. The X-T10 uses a several-years-old 16MP X-Trans APS-C sensor. It doesn't shoot 4K, or even offer particularly good HD video quality. Despite a valiant effort on the part of its engineers, it also can't reliably track subjects across the frame to keep them in focus no matter where they move to in continuous AF. </t>
+  </si>
+  <si>
+    <t>Fujifilm X-T10 Review</t>
+  </si>
+  <si>
+    <t>The answer is anyone looking for a digital camera that feels, handles and shoots like, well, an actual camera and not an electronic device. On paper, offerings from other brands like Sony, with the a6000, Nikon with the D5500 and Olympus with the O-MD E-M10 might seem more appealing or capable. When it comes to video, all of the above mentioned are more capable, and the same can generally be said for continuous focus modes outside of single-point AF-C. But from my experience having shot with all of these cameras, the X-T10 is hands down the most pleasurable of the bunch to use.
+Fujifilm makes cameras for people who love cameras, not specs. The X-T10 is a camera that will force you to slow down your shooting. That's not to say it doesn't make a good camera for shooting action. The 8 fps burst, while limited by its 1 sec buffer, works with the camera's AF system to keep focus on even rapidly moving subjects, provided you continuously reframe to keep your centrally-located AF point over your subject. I don't want to discredit the technology in the X-T10. As long as you manually select and use one of the 15 phase detect points located in the center of the frame, the camera is capable of acquiring and maintaining focus in most situations with moving targets. In single AF, it also finds and focuses on faces quite easily. Mirrorless means AF is also accurate. But at the same time, it's also extremely easy and pleasurable to focus manually.
+If you're really picky about having the most malleable Raw files possible, you might be better off looking to Nikon D5500 instead. That's not to say that X-T10's Raw files are crummy to work with, because they aren't, they're just not as well supported by third-party Raw converters as files from traditional Bayer-sensored competitors. That said, X-Trans punches above its 16MP weight when it comes to real-world resolution, and the usable dynamic range of Raw files from the X-T10 is still impressive, given the age of the (we believe Sony) sensor.
+The X-T10 is also very quiet, (silent when the electronic shutter is used) and is incredibly discreet to shoot with. The fold-out screen also makes for easy shooting-from-the-hip. And Face Detect greatly helps that act of shooting street photography of passersby. Unfortunately, it doesn't work all that well when shooting moving faces in AF-C. Fujifilm, if you're reading this, please fix this with a firmware update!
+Ergonomically, the X-T10 is light-weight, well-built and quite customizable. And let's face it, at the end of the day, one of the most important features of any camera is the desire it instills in you to pick it up and shoot. A camera that can be custom-tailored to your shooting style, with buttons and shortcut menus, will obviously make for a more engaging shooting experience.</t>
+  </si>
+  <si>
+    <t>Dan Bracaglia</t>
+  </si>
+  <si>
+    <t>https://cdn.builder.io/api/v1/image/assets%2F53e4b1c7e8314bb0af1a0d344422a86a%2F29bf2b97fb0c4ede99cd8b2a3844303d</t>
+  </si>
+  <si>
+    <t>Understanding how
+your sensor responds can open up creative options that aren't otherwise obvious. For instance, this high dynamic range scene was achieved using a single exposure, thanks to the camera's excellent noise characteristics.</t>
+  </si>
+  <si>
+    <t>Sources of camera
+noise part two: Electronic Noise</t>
+  </si>
+  <si>
+    <t>In the first part of this article, we discussed the fact that a lot of the noise in a lot of your images doesn't come from your camera at all: it is you being able to see the randomness of the light that you've captured and it is almost solely dependent on how much light you were able to capture. The second source of noise is more likely to resemble what most people think of, when they think of noise: it's the background electronic noise that's added to your images by the specific camera you're using. We say this is the source of noise that most people think of because it's much easier to think of noise the way you think of background 'hum' from a Hi-Fi amplifier.
+The key thing to remember though is that, although shot noise and electronic noise stem from very different sources, with the exception of a few special cases (such as 'banding' pattern noise), they are visually indistinguishable. Noise is just variation from the expected result: aberrantly brighter or darker pixels or spurious color.
+Just like with a Hi-Fi amplifier, you'll recognize that noise tends to be easier to hear during quiet patches in the music when you've got the volume turned up. In a similar manner, the electronic 'read noise' rumbles along in the dark tones of your image (where there isn't much signal) and is most likely to be visible when you've pushed your signal a lot (you're shooting at high ISO).
+To better understand the behavior of different sensors, we're going to split the sources of electronic noise into two groups and consider them separately. We're going to draw the line between noise added before amplification and any added afterwards. These come in addition to light's inherent shot noise that we covered in part one.
+What we're going to call Upstream read noise includes the electronic noise contributed by the pixel during the process of image capture*1. Downstream read noise includes the contribution of all the downstream electronics and all other sources after ISO amplification*2.
+The reason we'll look at these two sources separately is that, while they tend not to change very much (for any particular sensor), the upstream read noise has already been added to the signal before amplification, so gets amplified along with the signal when you change ISO, whereas downstream read noise stays the same, regardless of amplification. This difference becomes important when you compare performance between sensors, as it can dictate not only the results they give but also the most effective ways to use them.
+Most modern sensors have pretty low upstream read noise, the big differences between different sensor designs tend to be in how low the designers have managed to get the downstream read noise. For the rest of this article we're going to compare the behavior of two theoretical cameras: one with low upstream and low downstream read noise, and a second that differs by having higher downstream read noise, to see how and where their performance differs and consequently, how you should shoot with them. We've going to use the same tone flow diagrams that we used in part one of this article, tracking what happens to the tones in the scene, from the point of capture all the way into the final image.
+At low ISOs
+At base ISO, where there's no ISO amplification being applied, the low upstream read noise makes very little difference. However, the differences in downstream read noise can be seen in terms of low ISO dynamic range: a camera with lower downstream read noise will have greater low ISO dynamic range.
+There's every chance you won't see this in the camera's JPEGs, because even the noisiest contemporary cameras tend to have a noise floor below the darkest tone used in the JPEG. However, the best modern cameras can have several stops of additional usable dynamic range that you'll simply never see in your JPEGs. This is because JPEGs tend to have tone curves designed to create punchy images with plenty of contrast when displayed on monitors or as prints (which have relatively narrow dynamic ranges), but it means there are a lot of creative possibilities that open up if you want to shoot Raw and make use of this extra information (such as the image at the top of this page, which looked like this prior to a custom tone curve to bring out shadows).</t>
+  </si>
+  <si>
+    <t>Rishi Sanyal</t>
+  </si>
+  <si>
+    <t>13/05/2024</t>
+  </si>
+  <si>
+    <t>https://cdn.builder.io/api/v1/image/assets%2F53e4b1c7e8314bb0af1a0d344422a86a%2Fab61f61751c147899bed6438d46245e2</t>
+  </si>
+  <si>
+    <t>Aura Carver 10.1"
+digital photo frame review: A window to the photos you almost forgot</t>
+  </si>
+  <si>
+    <t>A step below tablets
+in functionality and offerings but more interactive and striking than a regular frame, digital frames are perennially giftable. What easier way to display photographs, including new ones sent digitally by friends and family? The Aura Carver 10.1" Wi-Fi Digital Picture Frame is a great choice, though not without flaws.</t>
+  </si>
+  <si>
+    <t>Powered by an AC adapter and proprietary cable, the frame is designed to be positioned in landscape orientation only, with the ability to display portrait images in pairs, side by side. The frame can also display videos but with some caveats.
+The screen is not a touchscreen (not that you'd want to be smudging it up with your fingers), but the frame has a touch strip along the top edge that you can use to swipe through photos and interact when necessary.
+Packaging and build
+I ran into my first two hurdles of the Carver unit right out of the box: its color and cord. The frame itself is an impressive and robust unit. It feels stable, sturdy, and professional. The Gravel (black) coloring, however, can scratch onto white surfaces. A white shelf or table, for example, may feature black scuff marks courtesy of the Carver when you set it up. The Carver also comes in Sea Salt (white), but if you'd prefer the black, the scuffs are nothing that a Magic Eraser or some caution can't solve.
+The Carver uses a unique power cord instead of a more standard variety like USB-C or Micro USB, and the unit also needs to be plugged in to run. Because you can't retract the cord or swap it out for a shorter or longer one, some cleverness may be required to keep your frame area neat and tidy.
+User Experience
+One of my mounted photograph prints watched jealously over my shoulder as I set up the entire Aura Carver digital frame in approximately 90 seconds, coming in under the two-minute estimate on the Aura website. This included downloading the app, linking the frame to my phone, and selecting photos to send over. You can spare your recipient part of this setup with Aura's gift mode, which allows you to pre-load some content and even a message that will display when they boot it up.
+The Carver frame defaults to slideshow mode, and you can select the length of time between each photo and video. Because the default is 10 minutes, I didn't realize slideshow mode was on in the first place. It can be configured to switch photos as quickly as a matter of seconds or up to 24 hours, depending on how quickly you want new photos to appear. Photographs look vibrant on the screen, and it's a joy to revisit pictures I would have otherwise forgotten.
+"It's a joy to revisit pictures I would have otherwise forgotten."
+While landscape photos fit the frame's aspect ratio, vertical photos do not and can be displayed side by side using Photo Pairing mode. As Aura explained to me for this review, photos are paired by the time when in Chronological Photo order, whereas, in Shuffle Photo Order, the photos are paired in a rough attempt by Aura's app to match the subject and location. You can also set a background for single vertical photos, either black or 'filled', which fills the negative space with a zoomed-in, out-of-focus version of the photo itself. When I selected 'filled', the treatment was not consistent for all of my shots, and some reverted to a black background.
+Videos have a hurdle of their own. When a video comes up on the unit, a 'Loading' progress bar appears on the screen with a 'Tap Touch Bar For Sound' at the top. The video is sometimes choppy upon playback and returns to a thumbnail at the end. It's functional but not particularly slick, so the Carver is best suited for portfolios that are heavy on still photos and light on videos.</t>
+  </si>
+  <si>
+    <t>Michelle DeLateur</t>
+  </si>
+  <si>
+    <t>21/06/2023</t>
+  </si>
+  <si>
+    <t>https://cdn.builder.io/api/v1/image/assets%2F53e4b1c7e8314bb0af1a0d344422a86a%2F2da9abbfe9954ba9b5bf78917ba11670</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +530,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -458,11 +566,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -782,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7B2FB6-0230-4029-B88F-3C4606A4A2E7}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1677,4 +1793,123 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A496E6-64AA-4D33-B6D6-8B80656E4CB6}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="6">
+        <v>45389</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{D37296FA-6523-43F8-986D-48324E7AB41E}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{EC5039B6-2208-4502-B22C-06C93B220F82}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{6B59912C-248B-4099-8411-37D6F34550D8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implemented sign-in/sign-up and product page UI; ongoing API integration and backend logic updates
</commit_message>
<xml_diff>
--- a/camera-shop/src/main/resources/data.xlsx
+++ b/camera-shop/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\camera-shop\camera-shop\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD03E976-967F-481D-8BD3-F74605A38F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD89CA3-5FD8-4E67-9305-4177397C7462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{90887BD4-D8A2-4FD5-939A-5967D6FE0B64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{90887BD4-D8A2-4FD5-939A-5967D6FE0B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Brand" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="229">
   <si>
     <t>id</t>
   </si>
@@ -242,14 +242,6 @@
 (Expandable: 50 to 51200)</t>
   </si>
   <si>
-    <t>Up to 11 fps at 
-24.2MP for up to 116 Frames (JPEG) / 46 Frames (RAW)</t>
-  </si>
-  <si>
-    <t>Digital (Video
-Only)</t>
-  </si>
-  <si>
     <t>cameraId</t>
   </si>
   <si>
@@ -307,15 +299,7 @@
     <t>RawXAVC HS, UHD 4K, 1920 x 1080p, 3840 x 2160</t>
   </si>
   <si>
-    <t>Speed Priority 
-Continuous Shooting: approx. 16fps, Continuous Shooting: approx. 3.5fps</t>
-  </si>
-  <si>
     <t>Approx. 20.1 Megapixels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Sony ZV-E1 is a versatile camera that 
-is well-suited for content creators. It is compact and lightweight, making it easy to carry around, and it features a full-frame sensor and powerful image processor that can capture high-quality images and videos. </t>
   </si>
   <si>
     <t>80 to 102,400 
@@ -325,9 +309,6 @@
     <t>Digital, 5-axis</t>
   </si>
   <si>
-    <t>Camera Only</t>
-  </si>
-  <si>
     <t>Camera + Grip</t>
   </si>
   <si>
@@ -356,9 +337,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719305543/camera/Sony%20ZV-E10/ae630dda-95ed-4be9-bc6b-2efe6e929fac.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719305555/camera/Sony%20ZV-E10/803943c0-2a6d-4e0e-842f-fce11f074f88.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305618/camera/Sony%20ZV-E10/394dd43e-7bf8-4633-8749-21c377a69dd0.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305568/camera/Sony%20ZV-E10/13192b7e-dea6-458c-b39d-4991927065e8.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305627/camera/Sony%20ZV-E10/8613dc9c-8ce2-4bf1-bac0-cd1eb7bd1e5d.png</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307531/camera/Sony%20ZV-E1/808593c8-c5ef-4fb4-a31c-506bc81b793e.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719307544/camera/Sony%20ZV-E1/f8bc95b0-d67d-4e21-90e1-9ed2d6db1e7a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307578/camera/Sony%20ZV-E1/a5d6be80-68f6-4d70-b4ec-c2aa84ab8919.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307578/camera/Sony%20ZV-E1/a5d6be80-68f6-4d70-b4ec-c2aa84ab8919.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307602/camera/Sony%20ZV-E1/91e001c1-d281-4f95-bd6c-3d3c30370122.png</t>
   </si>
   <si>
     <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307624/camera/Sony%20ZV-E1/17a716f9-9b1a-4fb0-8fb7-0d1d6a59ce41.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307640/camera/Sony%20ZV-E1/8017131e-93cb-44a8-ba40-c83655f1388e.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307615/camera/Sony%20ZV-E1/fb085051-4096-4f9e-a6a9-1ce5adb4d040.png</t>
@@ -435,10 +413,6 @@
   </si>
   <si>
     <t>https://cdn.builder.io/api/v1/image/assets%2F53e4b1c7e8314bb0af1a0d344422a86a%2F29bf2b97fb0c4ede99cd8b2a3844303d</t>
-  </si>
-  <si>
-    <t>Understanding how
-your sensor responds can open up creative options that aren't otherwise obvious. For instance, this high dynamic range scene was achieved using a single exposure, thanks to the camera's excellent noise characteristics.</t>
   </si>
   <si>
     <t>Sources of camera
@@ -468,10 +442,6 @@
   <si>
     <t>Aura Carver 10.1"
 digital photo frame review: A window to the photos you almost forgot</t>
-  </si>
-  <si>
-    <t>A step below tablets
-in functionality and offerings but more interactive and striking than a regular frame, digital frames are perennially giftable. What easier way to display photographs, including new ones sent digitally by friends and family? The Aura Carver 10.1" Wi-Fi Digital Picture Frame is a great choice, though not without flaws.</t>
   </si>
   <si>
     <t>Powered by an AC adapter and proprietary cable, the frame is designed to be positioned in landscape orientation only, with the ability to display portrait images in pairs, side by side. The frame can also display videos but with some caveats.
@@ -490,17 +460,337 @@
     <t>Michelle DeLateur</t>
   </si>
   <si>
-    <t>21/06/2023</t>
-  </si>
-  <si>
     <t>https://cdn.builder.io/api/v1/image/assets%2F53e4b1c7e8314bb0af1a0d344422a86a%2F2da9abbfe9954ba9b5bf78917ba11670</t>
+  </si>
+  <si>
+    <t>Fujifilm X-T4</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>Actual: 26.1 Megapixel (6240 x 4160)</t>
+  </si>
+  <si>
+    <t>DCI 4K (4096 x 2160) ; Full HD (1920 x 1080)</t>
+  </si>
+  <si>
+    <t>1 x NP-W235 Lithium-Ion, 7.2 VDC, 2200 mAh (600 shots)</t>
+  </si>
+  <si>
+    <t>134.6 x 92.8 x 63.8 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Sony ZV-E1 is a versatile camera that is well-suited for content creators. It is compact and lightweight, making it easy to carry around, and it features a full-frame sensor and powerful image processor that can capture high-quality images and videos. </t>
+  </si>
+  <si>
+    <t>Auto, ISO 160 to 12800 
+(Expandable: 80 to 51200)</t>
+  </si>
+  <si>
+    <t>Up to 15 fps at 26.1MP for up to 114 Frames (JPEG) / 36 Frames (RAW)</t>
+  </si>
+  <si>
+    <t>5-Axis Sensor-Shift</t>
+  </si>
+  <si>
+    <t>Canon EOS R6</t>
+  </si>
+  <si>
+    <t>The Canon EOS R6 offers both photographers and videographers a versatile and reliable camera body with impressive image quality and performance.</t>
+  </si>
+  <si>
+    <t>Auto, ISO 100 to 102400 (Expandable: 50 to 204800)</t>
+  </si>
+  <si>
+    <t>Up to 20 fps at 20.1MP for up to 240 Frames (JPEG) / 120 Frames (RAW)</t>
+  </si>
+  <si>
+    <t>Actual: 20.1 Megapixel (5472 x 3648)</t>
+  </si>
+  <si>
+    <t>1 x LP-E6NH Lithium-Ion, 7.2 VDC, 2130 mAh (510 shots)</t>
+  </si>
+  <si>
+    <t>526g</t>
+  </si>
+  <si>
+    <t>680g </t>
+  </si>
+  <si>
+    <t>138.4 x 97.5 x 88.4 mm</t>
+  </si>
+  <si>
+    <t>Nikon Z6 II</t>
+  </si>
+  <si>
+    <t>The Nikon Z6 II is a versatile mirrorless camera packed with powerful features for photographers and videographers alike.</t>
+  </si>
+  <si>
+    <t>Auto, ISO 100 to 51200 (Expandable: 50 to 204800)</t>
+  </si>
+  <si>
+    <t>Up to 14 fps at 24.5MP for up to 124 Frames (JPEG) / 34 Frames (RAW)</t>
+  </si>
+  <si>
+    <t>Actual: 24.5 Megapixel (6048 x 4024)</t>
+  </si>
+  <si>
+    <t>1 x EN-EL15c Lithium-Ion, 7.2 VDC, 2280 mAh (410 shots)</t>
+  </si>
+  <si>
+    <t>615g</t>
+  </si>
+  <si>
+    <t>134 x 100.5 x 69.5 mm</t>
+  </si>
+  <si>
+    <t>Leica Q2</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>The Leica Q2 is a compact, full-frame camera with a fixed lens, ideal for night and astrophotography with its high ISO performance and sharp optics.</t>
+  </si>
+  <si>
+    <t>Auto, ISO 50 to 50000</t>
+  </si>
+  <si>
+    <t>Up to 10 fps at 47.3MP</t>
+  </si>
+  <si>
+    <t>OIS</t>
+  </si>
+  <si>
+    <t>Actual: 47.3 Megapixel (8368 x 5584)</t>
+  </si>
+  <si>
+    <t>1 x BP-SCL4 Lithium-Ion, 7.4 VDC, 1860 mAh (370 shots)</t>
+  </si>
+  <si>
+    <t>718g</t>
+  </si>
+  <si>
+    <t>130 x 80 x 91.9 mm</t>
+  </si>
+  <si>
+    <t>Canon EOS M50 Mark II</t>
+  </si>
+  <si>
+    <t>The Canon EOS M50 Mark II is a versatile and compact mirrorless camera perfect for travel and everyday photography with its APS-C sensor and advanced features.</t>
+  </si>
+  <si>
+    <t>Auto, ISO 100 to 25600 (Expandable: 100 to 51200)</t>
+  </si>
+  <si>
+    <t>Up to 10 fps at 24.1MP for up to 33 Frames (JPEG) / 10 Frames (RAW)</t>
+  </si>
+  <si>
+    <t>Digital (Video Only)</t>
+  </si>
+  <si>
+    <t>Actual: 24.1 Megapixel (6000 x 4000)</t>
+  </si>
+  <si>
+    <t>APS-C</t>
+  </si>
+  <si>
+    <t>UHD 4K (3840 x 2160); Full HD (1920 x 1080)</t>
+  </si>
+  <si>
+    <t>1 x LP-E12 Lithium-Ion, 7.2 VDC, 875 mAh (305 shots)</t>
+  </si>
+  <si>
+    <t>387g</t>
+  </si>
+  <si>
+    <t>116.3 x 88.1 x 58.7 mm</t>
+  </si>
+  <si>
+    <t>Nikon Z7 II</t>
+  </si>
+  <si>
+    <t>The Nikon Z7 II is a high-resolution full-frame mirrorless camera designed for expert and studio photographers, offering exceptional image quality and performance.</t>
+  </si>
+  <si>
+    <t>Auto, ISO 64 to 25600 (Expandable: 32 to 102400)</t>
+  </si>
+  <si>
+    <t>Up to 10 fps at 45.7MP for up to 50 Frames (RAW)</t>
+  </si>
+  <si>
+    <t>Actual: 45.7 Megapixel (8256 x 5504)</t>
+  </si>
+  <si>
+    <t>Full-Frame</t>
+  </si>
+  <si>
+    <t>1 x EN-EL15c Lithium-Ion, 7.0 VDC, 2280 mAh (420 shots)</t>
+  </si>
+  <si>
+    <t>705g</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721130636/camera/Fujifilm%20X-T4/99c9cd23-cfb7-4fcd-b1a9-2629aa37a94e.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130673/camera/Fujifilm%20X-T4/bf88c7fe-0512-48d1-8328-ee71c14d63de.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130687/camera/Fujifilm%20X-T4/b4d0510e-94c4-4b02-b3df-a81c04b0ea60.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130700/camera/Fujifilm%20X-T4/9f833926-3d53-4e2f-bcdd-4e8c605412bb.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130703/camera/Fujifilm%20X-T4/df498503-022a-431f-b230-324d59ee7b7a.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721130793/camera/Canon%20EOS%20R6/ffd9df59-29e1-4e9e-8d73-c941398ef273.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130808/camera/Canon%20EOS%20R6/423e0de6-ff10-49f1-9f66-94c844938f8f.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130819/camera/Canon%20EOS%20R6/158754ff-14f9-47f3-958c-4224aa56975f.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130825/camera/Canon%20EOS%20R6/43671d1e-c344-4921-989c-510006cb595d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130847/camera/Canon%20EOS%20R6/e3639221-082f-4dd2-bfca-d97cf55c0944.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721130896/camera/Nikon%20Z6%20II/c5a8fe49-4ccf-4962-8b6a-a16c881a1c5a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130906/camera/Nikon%20Z6%20II/1ba46d9d-a04c-4bc0-9fde-03f6d46329f1.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130911/camera/Nikon%20Z6%20II/ddc79460-9337-458d-878a-7c9254c67eff.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130932/camera/Nikon%20Z6%20II/0b258bbf-e600-4fa2-b274-640fd330c9cb.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130937/camera/Nikon%20Z6%20II/ac11b8c9-8994-4927-96d4-87f3a916d325.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721131052/camera/Leica%20Q2/a1614e9a-7c82-47ab-8538-0cf546cf162d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131052/camera/Leica%20Q2/a1614e9a-7c82-47ab-8538-0cf546cf162d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131058/camera/Leica%20Q2/c9c25964-dda5-4170-91ed-b77f819de908.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131065/camera/Leica%20Q2/d5522030-38b2-4a4f-b31b-477500938282.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131067/camera/Leica%20Q2/7bc53414-d61e-439a-9ada-d3f8e2dc0728.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721136732/camera/Canon%20EOS%20M50%20Mark%20II/77661828-f6e0-4def-b5c7-b3b39efd4664.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721136738/camera/Canon%20EOS%20M50%20Mark%20II/d5672eff-2b71-49f4-bd7a-ef91c6b111b9.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721136757/camera/Canon%20EOS%20M50%20Mark%20II/62a8f012-f76f-4f23-b10e-5f603f13543c.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721136765/camera/Canon%20EOS%20M50%20Mark%20II/8cca4d49-5244-465e-9fa5-0c13bbb78f6e.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721136835/camera/Nikon%20Z7%20II/742a344d-cb29-48fb-af71-2cdb4aca4b3d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721136839/camera/Nikon%20Z7%20II/ef8da171-e7b3-493e-84ac-6db01134bcf8.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721136854/camera/Nikon%20Z7%20II/6306a986-7ee6-48a7-8045-58d690f4530c.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721136876/camera/Nikon%20Z7%20II/20038629-3004-4cb2-9393-3b90596c8cd5.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721136885/camera/Nikon%20Z7%20II/945fa9ae-222b-4b00-bd9e-0924a1852ff4.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721137077/camera/Fujifilm%20X-T4/c47fdb92-6856-4c3e-85ed-763f3288bba7.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721137097/camera/Fujifilm%20X-T4/bd0f4908-7c8c-4ac1-b767-75521a31a1fc.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721137088/camera/Fujifilm%20X-T4/fa63775e-9a0a-4a08-b2fb-aa1f6ee2a043.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721137082/camera/Fujifilm%20X-T4/c74b0398-17f0-4c9e-8fe1-792dfcd7fcde.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721137104/camera/Fujifilm%20X-T4/29400c68-340c-4d8e-a9a1-f7dc9494b4a2.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721137676/camera/Fujifilm%20X-T4/e05aac44-84ab-4226-9f13-7a84bac2982d.png</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721137797/camera/Fujifilm%20X-T4/e428ffa6-0af5-4ac9-9d9e-c587c2e1c5a3.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721137825/camera/Fujifilm%20X-T4/75a3f5de-f069-44d3-a132-b4dadb21fe43.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721137838/camera/Fujifilm%20X-T4/ed4ef32f-44e3-4bca-97ce-aa6d3c566700.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721137943/camera/Fujifilm%20X-T4/eec4e0c7-02a6-48d1-94f7-82db824ebe50.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721137835/camera/Fujifilm%20X-T4/256e81a9-76f6-4ec6-aaca-9a6b02b3b0c7.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721137946/camera/Fujifilm%20X-T4/9f543d9c-37bc-4391-ad16-59ad5e7c31a2.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721138272/camera/Canon%20EOS%20R6/e259bcf6-bf08-4994-a31f-7f4806bc91d3.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721138280/camera/Canon%20EOS%20R6/67ff3226-03be-4a3d-a41c-c498a63d3a7f.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721138289/camera/Canon%20EOS%20R6/65936270-bdb4-485d-b7d5-d6d3fa06af9c.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721138294/camera/Canon%20EOS%20R6/6a407e1d-b692-4001-8f65-babdb064a22a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721138483/camera/Canon%20EOS%20R6/977fa43f-1f56-436a-93f3-768de74cead9.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721138486/camera/Canon%20EOS%20R6/26cf6932-190b-45e7-aaad-99689914c59b.png</t>
+  </si>
+  <si>
+    <t>Lens 24-105mm f/4-7.1</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721138568/camera/Canon%20EOS%20R6/d87e1377-073d-4c2a-94df-ebfb0a44f96c.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721138757/camera/Canon%20EOS%20R6/5965227a-9155-4bec-baf1-b72f95f20ba5.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721138576/camera/Canon%20EOS%20R6/f34db8ca-6838-4290-b20b-f462f432892d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721138760/camera/Canon%20EOS%20R6/15bdc9f8-8197-4d2a-9539-b1ac08f4a5c5.png</t>
+  </si>
+  <si>
+    <t>Body Only</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721138955/camera/Nikon%20Z6%20II/d594f74b-5d94-4466-964e-1bd1ab45f5e5.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721138987/camera/Nikon%20Z6%20II/d7ebe26a-7e6f-4b69-aba5-3e606645d0e4.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721138985/camera/Nikon%20Z6%20II/ca25c9f0-b03e-4bd9-bcf5-5bb0d2b925e9.png</t>
+  </si>
+  <si>
+    <t>Lens Z 24-70mm F4/s</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721139117/camera/Nikon%20Z6%20II/9eab0654-98fc-4e88-b15e-e40bd7d6e05e.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139136/camera/Nikon%20Z6%20II/e4cfae06-f8c8-455c-bd0a-45006696a031.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139149/camera/Nikon%20Z6%20II/aa845562-407e-474a-89c6-d4083f15602f.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139133/camera/Nikon%20Z6%20II/5267bd62-5c8a-4762-b1ef-0a96c042d3b9.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721139211/camera/Leica%20Q2/385a7fc9-20c1-4c73-8ff9-8f7290656fe9.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139218/camera/Leica%20Q2/3e0c23ee-ec0b-4297-b53e-92e316a697c0.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139281/camera/Leica%20Q2/c0ec1359-3db4-4a45-927b-5b9c96c6d170.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139352/camera/Leica%20Q2/192d9e0d-1330-4986-b1cc-71996c654dfe.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139226/camera/Leica%20Q2/a9d21b84-dc28-48a7-a80c-a2f4126aafbe.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139343/camera/Leica%20Q2/d00ee826-0d65-43f3-a771-88f3d11c121a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139346/camera/Leica%20Q2/7b769224-a2a3-4287-94c2-adc7778e4871.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139349/camera/Leica%20Q2/36cfe5f7-aa47-4ea4-b6bb-8e125fed7d1e.png</t>
+  </si>
+  <si>
+    <t>Kit 15-45mm f/3.5-6.3 IS</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721139687/camera/Canon%20EOS%20M50%20Mark%20II/3b5a79de-d67c-4eb3-9689-ce81d3c83f9e.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139714/camera/Canon%20EOS%20M50%20Mark%20II/68c1a038-5676-48e1-b562-e8144b8cf59e.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139950/camera/Canon%20EOS%20M50%20Mark%20II/bb7cebf0-4713-4867-aa91-6473701b712d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139717/camera/Canon%20EOS%20M50%20Mark%20II/ae18f09a-6f8b-44ab-8509-4b2bb085a7db.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721139915/camera/Canon%20EOS%20M50%20Mark%20II/2445da2a-ec2c-4a17-a152-d4c2c7b764dd.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139888/camera/Canon%20EOS%20M50%20Mark%20II/038f9b2d-abe3-4444-8ae7-317ed7e60bb9.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139877/camera/Canon%20EOS%20M50%20Mark%20II/8afeb28a-4f4c-472e-9baf-bcee70a26871.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139892/camera/Canon%20EOS%20M50%20Mark%20II/ba37762f-d856-4be3-bdc4-354284f3c1a7.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721140172/camera/Nikon%20Z7%20II/391f81d5-4663-44f9-82e6-8307c99d79f9.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721140188/camera/Nikon%20Z7%20II/4a022a03-7f7a-4380-870b-652a9a2b64fa.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721140211/camera/Nikon%20Z7%20II/61bf1485-1383-43c0-beb3-66a7e162f864.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721140195/camera/Nikon%20Z7%20II/a93fa98d-6f65-461d-9bc2-07d34cfb7e18.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721140192/camera/Nikon%20Z7%20II/5daecc9c-e3f0-4723-9be9-d86957291fde.png</t>
+  </si>
+  <si>
+    <t>Lens 24-70mm f4</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721140358/camera/Nikon%20Z7%20II/c8e20764-0a52-4656-955f-12587a728964.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721140372/camera/Nikon%20Z7%20II/dcf5e560-3c08-4831-be60-4f5c1d639c93.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721140379/camera/Nikon%20Z7%20II/b6c9d211-3339-491d-94ad-2c050475a7a2.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721140383/camera/Nikon%20Z7%20II/06b3f8f8-81ff-4907-992a-4fe44c5781ac.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721140387/camera/Nikon%20Z7%20II/0106322a-9d9b-4394-a98d-8b929cd827cc.png</t>
+  </si>
+  <si>
+    <t>By way of its strategic partnership with Huawei, Leica is already involved in the development of smartphone camera technology. However, it appears chairman of the supervisory board Andreas Kaufmann can imagine the German manufacturer taking things one step further and making its own camera phone.</t>
+  </si>
+  <si>
+    <t>Leica Smartphone: A Niche Market with a Premium Touch?</t>
+  </si>
+  <si>
+    <t>Leica's ambitions for a smartphone go beyond simply entering the saturated market. While most brands focus on features and specs, Leica seeks to reclaim the art of photography. Kaufmann envisions a device meticulously designed for capturing the essence of a moment, prioritizing quality over quantity.
+Imagine a Leica smartphone boasting a unique ergonomic grip, specifically tailored for landscape photography. Its lens, crafted with Leica's renowned expertise, could offer unparalleled image quality and depth, rivaling even dedicated cameras.
+The interface would be refined, prioritizing control over automation, allowing seasoned photographers to fine-tune every aspect of their shot. A dedicated shutter button, reminiscent of traditional cameras, would ensure a more tactile and deliberate shooting experience.
+However, achieving this vision comes with its own challenges. The smartphone market is highly competitive, with giants like Apple and Samsung already dominating the scene. Leica's success would hinge on attracting a dedicated audience willing to pay a premium for a smartphone built for photography enthusiasts.
+Ultimately, the success of a Leica smartphone boils down to the company's ability to create a device that truly embodies its legacy of quality and artistry. While the market may be skeptical, a dedicated niche of photographers eager for a superior photographic experience could be the key to Leica's foray into the smartphone world.</t>
+  </si>
+  <si>
+    <t>Lars Rehm</t>
+  </si>
+  <si>
+    <t>21/06/2024</t>
+  </si>
+  <si>
+    <t>https://cdn.builder.io/api/v1/image/assets%2F53e4b1c7e8314bb0af1a0d344422a86a%2F867c2e1b367e48fe8f1cfdaa931e518f</t>
+  </si>
+  <si>
+    <t>6 Best high-end cameras</t>
+  </si>
+  <si>
+    <t>Once you venture above $2500, you gain access to some extremely capable cameras. These are the models that deliver the highest levels of detail, some of the most sophisticated video features, high burst rates or a combination of all three.</t>
+  </si>
+  <si>
+    <t>Once you venture above $2500, you gain access to some extremely capable cameras. These are the models that deliver the highest levels of detail, some of the most sophisticated video features, high burst rates or a combination of all three.
+For most applications, the cameras around $2000 are excellent, but if you and your photography need the very highest image quality or some specialist capability, the cameras in this guide are among the best we've yet seen. There are a handful of dedicated sports/photojournalism cameras or luxury models above the $4000 upper limit we've set ourselves, but these are usually such singular offerings that we're assuming you don't need our help in choosing if you're seriously considering them.
+It's notable that there's no such thing as a bad camera at this level, so if you have any investment at all in the lens system of one company (or plan to adapt DSLR-era lenses from them), this should probably be the deciding factor for you. But we'll highlight the particular strengths we found in each camera, just in case you are planning to switch systems.
+Best high-end camera: Nikon Z8
+The Nikon Z8 is a fast-shooting stills and video-capable mirrorless camera with a 46MP Stacked CMOS sensor.
+The Z8 has a large, comfortable grip with well-placed controls. There's a good level of customizable controls and ergonomics that match the pro-focused Z9. The viewfinder resolution is low but the brightness and lack of lag make it one of best-suited to action.
+The Z8 can be set to track whatever's under the AF point and does so dependably. It can also prioritize recognized subjects near the AF point if you prefer. 20fps Raw shooting or 30fps full-res JPEG capture (with pre-burst option) make the Z8 very rapid.
+The compact option: Sony a7CR
+The Sony a7CR is a compact, full-frame camera with a 61MP BSI CMOS sensor. Despite its small size, it packs in most of the features found in Sony’s larger bodies while still delivering stunning detail, without sacrificing much performance.
+The a7CR is impressively small for a full-frame camera. The addition of a front control dial improves handling significantly. Notably, there’s no joystick for positioning the AF point, and the viewfinder is small and very low resolution for a camera costing this much.
+A capable Canon: Canon EOS R5
+The Canon EOS R5 is a versatile and capable full-frame mirrorless camera that can shoot 45 megapixel stills at up to 20 frames per second and capture 8K video.
+The Canon EOS R5 offers great image quality and very solid AF but the arrival of the Nikon Z8 starts to show the weaker points in its spec: its 20fps mode uses electronic shutter which isn't especially fast to read out, risking rolling shutter. Likewise the video looks great but the HQ 4K mode, taken from 8K capture, and 8K itself can prompt the camera to overheat fairly readily, and it can't shoot either at 60p as the Nikon can.
+Its high degree of backward compatibility is a major factor in its appeal, even if it's a little behind its rivals in some respects. If you have any significant committment to high-end Canon EF DSLR lenses, the EOS R5 will offer the most consistent performance with them.
+High-spec high res: Sony a7R V
+The Sony a7R V is the company's fifth-generation high-res full-frame mirrorless camera, built around a stabilized 61MP sensor.
+The Sony a7R V is focused more on high resolution than the combination of resolution and speed that the Nikon Z8 (and, to a lesser extent, the Canon EOS R5) offers. It can shoot 8K video but only with a major crop and significant rolling shutter.
+IQ above all else: Fujifilm GFX 50S II
+The Fujifilm GFX 50S II is a (relatively) compact 50MP medium format mirrorless interchangeable lens camera with built-in image stabilization.
+Fujifilm's most affordable medium format camera is a highly attractive option for enthusiasts and professionals alike.
+The 50S II is the least expensive digital medium format camera ever launched. Image stabilization and precise focus extend its usability far beyond the studio. Speed, autofocus and video aren't its greatest strengths, but it should have major appeal for enthusiast photographers wanting some of the best image quality available.
+Best for video: Sony FX3
+The Sony FX3 is part of Sony's Cinema line of cameras, but we've included it here because it shares so much in common with the a7S III, but is a better choice, we feel.
+The Sony FX3 is an image-stabilized, fan-cooled full-frame video camera designed to shoot UHD 4K footage at up to 120p.
+It loses out on a viewfinder, compared to the a7S III, but gains dependability and extended recording times thanks to the addition of a cooling fan. It appears to cost a little more on paper but the FX3 comes with a top handle with built-in XLR adapters, which is an expensive add-on to the a7S III. Sony has also added some video-centric features, such as EI exposure to the FX3 that haven't then appeared on its more stills-focused cameras.</t>
+  </si>
+  <si>
+    <t>Dpreview staff</t>
+  </si>
+  <si>
+    <t>13/07/2024</t>
+  </si>
+  <si>
+    <t>https://cdn.builder.io/api/v1/image/assets%2F53e4b1c7e8314bb0af1a0d344422a86a%2F91b1d925f4f44fb8b26a03ccdcb7f6f6</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721141649/camera/Canon%20EOS%20M50%20Mark%20II/c9ab6372-dacf-40d2-8c6c-cedd0b7f4e18.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721139518/camera/Canon%20EOS%20M50%20Mark%20II/209b85fb-a851-43a0-994a-0a261001af7e.png</t>
+  </si>
+  <si>
+    <t>Up to 11 fps at 24.2MP for up to 116 Frames (JPEG) / 46 Frames (RAW)</t>
+  </si>
+  <si>
+    <t>Speed Priority Continuous Shooting: approx. 16fps, Continuous Shooting: approx. 3.5fps</t>
+  </si>
+  <si>
+    <t>The Fujifilm X-T4 is a powerful mirrorless camera that combines a robust, weather-sealed body with professional features for both photo and video.</t>
+  </si>
+  <si>
+    <t>A step below tablets in functionality and offerings but more interactive and striking than a regular frame, digital frames are perennially giftable. What easier way to display photographs, including new ones sent digitally by friends and family? The Aura Carver 10.1" Wi-Fi Digital Picture Frame is a great choice, though not without flaws.</t>
+  </si>
+  <si>
+    <t>Understanding how your sensor responds can open up creative options that aren't otherwise obvious. For instance, this high dynamic range scene was achieved using a single exposure, thanks to the camera's excellent noise characteristics.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307531/camera/Sony%20ZV-E1/808593c8-c5ef-4fb4-a31c-506bc81b793e.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719307544/camera/Sony%20ZV-E1/f8bc95b0-d67d-4e21-90e1-9ed2d6db1e7a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307578/camera/Sony%20ZV-E1/a5d6be80-68f6-4d70-b4ec-c2aa84ab8919.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307602/camera/Sony%20ZV-E1/91e001c1-d281-4f95-bd6c-3d3c30370122.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,10 +829,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF222222"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -566,7 +863,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -574,11 +871,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -899,7 +1203,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -935,7 +1239,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -952,7 +1256,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -969,7 +1273,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -986,7 +1290,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -1003,7 +1307,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -1029,7 +1333,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1066,7 +1370,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
         <v>43</v>
@@ -1083,7 +1387,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
@@ -1100,7 +1404,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
         <v>51</v>
@@ -1117,7 +1421,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
@@ -1134,7 +1438,7 @@
         <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
         <v>53</v>
@@ -1151,7 +1455,7 @@
         <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
@@ -1168,7 +1472,7 @@
         <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>55</v>
@@ -1196,7 +1500,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1279,24 +1583,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DE6A29-D1BE-4327-A15B-C071AAA1973B}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
     <col min="3" max="3" width="7.77734375" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="35.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="40.88671875" customWidth="1"/>
@@ -1308,7 +1612,7 @@
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1327,16 +1631,16 @@
       <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1384,19 +1688,19 @@
         <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>66</v>
+        <v>223</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="K2" t="s">
         <v>57</v>
@@ -1420,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -1431,7 +1735,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1443,45 +1747,399 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J3" t="s">
-        <v>91</v>
-      </c>
       <c r="K3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L3" t="s">
         <v>59</v>
       </c>
       <c r="M3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="72.599999999999994" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" t="s">
+        <v>134</v>
+      </c>
+      <c r="N4" t="s">
+        <v>135</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="P4" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="72.599999999999994" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K5" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" t="s">
+        <v>146</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="P5" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>188</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="K7" t="s">
+        <v>164</v>
+      </c>
+      <c r="L7" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="P7" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="L8" t="s">
+        <v>174</v>
+      </c>
+      <c r="M8" t="s">
+        <v>175</v>
+      </c>
+      <c r="N8" t="s">
+        <v>176</v>
+      </c>
+      <c r="O8" t="s">
+        <v>177</v>
+      </c>
+      <c r="P8" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="N9" t="s">
+        <v>185</v>
+      </c>
+      <c r="O9" t="s">
+        <v>186</v>
+      </c>
+      <c r="P9" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="S9">
         <v>1</v>
       </c>
     </row>
@@ -1489,6 +2147,7 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1719304295/camera/Sony%20ZV-E10/1.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304305/camera/Sony%20ZV-E10/2.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304320/camera/Sony%20ZV-E10/3.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304338/camera/Sony%20ZV-E10/4.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304352/camera/Sony%20ZV-E10/5.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304360/camera/Sony%20ZV-E10/6.png" xr:uid="{9EBC3287-3930-410E-98A8-BAE127E2D274}"/>
+    <hyperlink ref="R4" r:id="rId2" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1721130636/camera/Fujifilm X-T4/99c9cd23-cfb7-4fcd-b1a9-2629aa37a94e.png" xr:uid="{244D9906-E6AB-41F5-B102-06D09B101306}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1496,21 +2155,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D78C07-7927-4BB8-A0DC-CDDE00B048CF}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="13.5546875" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1"/>
     <col min="6" max="6" width="21.77734375" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="10" width="24.77734375" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
     <col min="11" max="11" width="8.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1519,28 +2178,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>41</v>
@@ -1557,16 +2216,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
         <v>77</v>
-      </c>
-      <c r="D2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>79</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -1578,7 +2237,7 @@
         <v>950</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1592,16 +2251,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
         <v>78</v>
-      </c>
-      <c r="E3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" t="s">
-        <v>80</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -1613,7 +2272,7 @@
         <v>1300</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1627,16 +2286,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
         <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" t="s">
-        <v>79</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -1648,7 +2307,7 @@
         <v>950</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1662,13 +2321,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>199</v>
       </c>
       <c r="G5">
         <v>7</v>
@@ -1680,7 +2339,7 @@
         <v>620</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>103</v>
+        <v>228</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -1694,13 +2353,13 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
         <v>78</v>
-      </c>
-      <c r="E6" t="s">
-        <v>80</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1712,7 +2371,7 @@
         <v>950</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -1726,13 +2385,13 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>199</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -1744,7 +2403,7 @@
         <v>620</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1758,13 +2417,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G8">
         <v>8</v>
@@ -1776,9 +2435,396 @@
         <v>770</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1260</v>
+      </c>
+      <c r="J9" t="s">
+        <v>193</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" t="s">
+        <v>199</v>
+      </c>
+      <c r="F10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1380</v>
+      </c>
+      <c r="J10" t="s">
+        <v>195</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" t="s">
+        <v>199</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>1480</v>
+      </c>
+      <c r="J11" t="s">
+        <v>196</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" t="s">
+        <v>197</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>3800</v>
+      </c>
+      <c r="J12" t="s">
+        <v>198</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
+        <v>199</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>1500</v>
+      </c>
+      <c r="J13" t="s">
+        <v>200</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>15</v>
+      </c>
+      <c r="I14">
+        <v>2050</v>
+      </c>
+      <c r="J14" t="s">
+        <v>202</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>5100</v>
+      </c>
+      <c r="J15" t="s">
+        <v>203</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" t="s">
+        <v>199</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>15</v>
+      </c>
+      <c r="I16">
+        <v>500</v>
+      </c>
+      <c r="J16" t="s">
+        <v>222</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
+        <v>204</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+      <c r="I17">
+        <v>550</v>
+      </c>
+      <c r="J17" t="s">
+        <v>206</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" t="s">
+        <v>204</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>20</v>
+      </c>
+      <c r="I18">
+        <v>550</v>
+      </c>
+      <c r="J18" t="s">
+        <v>205</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" t="s">
+        <v>199</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19">
+        <v>2200</v>
+      </c>
+      <c r="J19" t="s">
+        <v>207</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" t="s">
+        <v>208</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>15</v>
+      </c>
+      <c r="I20">
+        <v>2900</v>
+      </c>
+      <c r="J20" t="s">
+        <v>209</v>
+      </c>
+      <c r="K20">
         <v>1</v>
       </c>
     </row>
@@ -1797,10 +2843,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A496E6-64AA-4D33-B6D6-8B80656E4CB6}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1817,19 +2863,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>4</v>
@@ -1840,22 +2886,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="6">
+        <v>120</v>
+      </c>
+      <c r="F2" s="5">
         <v>45389</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -1863,22 +2909,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>128</v>
+        <v>227</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>133</v>
+        <v>125</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -1886,22 +2932,68 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>135</v>
+        <v>226</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>139</v>
+        <v>214</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="10">
+        <v>45603</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -1909,6 +3001,8 @@
     <hyperlink ref="G2" r:id="rId1" xr:uid="{D37296FA-6523-43F8-986D-48324E7AB41E}"/>
     <hyperlink ref="G3" r:id="rId2" xr:uid="{EC5039B6-2208-4502-B22C-06C93B220F82}"/>
     <hyperlink ref="G4" r:id="rId3" xr:uid="{6B59912C-248B-4099-8411-37D6F34550D8}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{7984D2C1-1240-4AE4-BF31-9A6C38B4374D}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{782DCD0D-478D-4CDC-811C-4E2B8F65ACEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement cart item addition and order creation
</commit_message>
<xml_diff>
--- a/camera-shop/src/main/resources/data.xlsx
+++ b/camera-shop/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\camera-shop\camera-shop\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD89CA3-5FD8-4E67-9305-4177397C7462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050D0733-2656-4EA0-8A2A-AB2D26279F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{90887BD4-D8A2-4FD5-939A-5967D6FE0B64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{90887BD4-D8A2-4FD5-939A-5967D6FE0B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Brand" sheetId="1" r:id="rId1"/>
@@ -641,9 +641,6 @@
     <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721130896/camera/Nikon%20Z6%20II/c5a8fe49-4ccf-4962-8b6a-a16c881a1c5a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130906/camera/Nikon%20Z6%20II/1ba46d9d-a04c-4bc0-9fde-03f6d46329f1.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130911/camera/Nikon%20Z6%20II/ddc79460-9337-458d-878a-7c9254c67eff.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130932/camera/Nikon%20Z6%20II/0b258bbf-e600-4fa2-b274-640fd330c9cb.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721130937/camera/Nikon%20Z6%20II/ac11b8c9-8994-4927-96d4-87f3a916d325.png</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721131052/camera/Leica%20Q2/a1614e9a-7c82-47ab-8538-0cf546cf162d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131052/camera/Leica%20Q2/a1614e9a-7c82-47ab-8538-0cf546cf162d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131058/camera/Leica%20Q2/c9c25964-dda5-4170-91ed-b77f819de908.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131065/camera/Leica%20Q2/d5522030-38b2-4a4f-b31b-477500938282.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131067/camera/Leica%20Q2/7bc53414-d61e-439a-9ada-d3f8e2dc0728.png</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721136732/camera/Canon%20EOS%20M50%20Mark%20II/77661828-f6e0-4def-b5c7-b3b39efd4664.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721136738/camera/Canon%20EOS%20M50%20Mark%20II/d5672eff-2b71-49f4-bd7a-ef91c6b111b9.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721136757/camera/Canon%20EOS%20M50%20Mark%20II/62a8f012-f76f-4f23-b10e-5f603f13543c.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721136765/camera/Canon%20EOS%20M50%20Mark%20II/8cca4d49-5244-465e-9fa5-0c13bbb78f6e.png</t>
   </si>
   <si>
@@ -784,6 +781,9 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307531/camera/Sony%20ZV-E1/808593c8-c5ef-4fb4-a31c-506bc81b793e.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719307544/camera/Sony%20ZV-E1/f8bc95b0-d67d-4e21-90e1-9ed2d6db1e7a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307578/camera/Sony%20ZV-E1/a5d6be80-68f6-4d70-b4ec-c2aa84ab8919.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307602/camera/Sony%20ZV-E1/91e001c1-d281-4f95-bd6c-3d3c30370122.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721131052/camera/Leica%20Q2/a1614e9a-7c82-47ab-8538-0cf546cf162d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131058/camera/Leica%20Q2/c9c25964-dda5-4170-91ed-b77f819de908.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131065/camera/Leica%20Q2/d5522030-38b2-4a4f-b31b-477500938282.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131067/camera/Leica%20Q2/7bc53414-d61e-439a-9ada-d3f8e2dc0728.png</t>
   </si>
 </sst>
 </file>
@@ -1585,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DE6A29-D1BE-4327-A15B-C071AAA1973B}">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="K3" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1697,7 +1697,7 @@
         <v>65</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>172</v>
@@ -1756,7 +1756,7 @@
         <v>86</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>87</v>
@@ -1809,7 +1809,7 @@
         <v>132</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>138</v>
@@ -2018,8 +2018,8 @@
       <c r="Q7">
         <v>1</v>
       </c>
-      <c r="R7" s="3" t="s">
-        <v>190</v>
+      <c r="R7" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="S7">
         <v>1</v>
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -2137,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="S9">
         <v>1</v>
@@ -2148,6 +2148,7 @@
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1719304295/camera/Sony%20ZV-E10/1.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304305/camera/Sony%20ZV-E10/2.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304320/camera/Sony%20ZV-E10/3.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304338/camera/Sony%20ZV-E10/4.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304352/camera/Sony%20ZV-E10/5.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304360/camera/Sony%20ZV-E10/6.png" xr:uid="{9EBC3287-3930-410E-98A8-BAE127E2D274}"/>
     <hyperlink ref="R4" r:id="rId2" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1721130636/camera/Fujifilm X-T4/99c9cd23-cfb7-4fcd-b1a9-2629aa37a94e.png" xr:uid="{244D9906-E6AB-41F5-B102-06D09B101306}"/>
+    <hyperlink ref="R7" r:id="rId3" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1721131052/camera/Leica%20Q2/a1614e9a-7c82-47ab-8538-0cf546cf162d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131058/camera/Leica%20Q2/c9c25964-dda5-4170-91ed-b77f819de908.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131065/camera/Leica%20Q2/d5522030-38b2-4a4f-b31b-477500938282.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131067/camera/Leica%20Q2/7bc53414-d61e-439a-9ada-d3f8e2dc0728.png" xr:uid="{302D02AB-12FB-4CA3-BC27-F302994B1DF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2157,7 +2158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D78C07-7927-4BB8-A0DC-CDDE00B048CF}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2327,7 +2328,7 @@
         <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G5">
         <v>7</v>
@@ -2339,7 +2340,7 @@
         <v>620</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -2391,7 +2392,7 @@
         <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -2455,7 +2456,7 @@
         <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F9" t="s">
         <v>77</v>
@@ -2470,7 +2471,7 @@
         <v>1260</v>
       </c>
       <c r="J9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -2487,10 +2488,10 @@
         <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F10" t="s">
         <v>77</v>
@@ -2505,7 +2506,7 @@
         <v>1380</v>
       </c>
       <c r="J10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -2525,7 +2526,7 @@
         <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G11">
         <v>5</v>
@@ -2537,7 +2538,7 @@
         <v>1480</v>
       </c>
       <c r="J11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -2557,7 +2558,7 @@
         <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2569,7 +2570,7 @@
         <v>3800</v>
       </c>
       <c r="J12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -2589,7 +2590,7 @@
         <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -2601,7 +2602,7 @@
         <v>1500</v>
       </c>
       <c r="J13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -2621,7 +2622,7 @@
         <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -2633,7 +2634,7 @@
         <v>2050</v>
       </c>
       <c r="J14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -2662,7 +2663,7 @@
         <v>5100</v>
       </c>
       <c r="J15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -2682,7 +2683,7 @@
         <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -2694,7 +2695,7 @@
         <v>500</v>
       </c>
       <c r="J16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -2714,7 +2715,7 @@
         <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -2726,7 +2727,7 @@
         <v>550</v>
       </c>
       <c r="J17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -2746,7 +2747,7 @@
         <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2758,7 +2759,7 @@
         <v>550</v>
       </c>
       <c r="J18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2778,7 +2779,7 @@
         <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G19">
         <v>3</v>
@@ -2790,7 +2791,7 @@
         <v>2200</v>
       </c>
       <c r="J19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -2810,7 +2811,7 @@
         <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -2822,7 +2823,7 @@
         <v>2900</v>
       </c>
       <c r="J20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -2912,7 +2913,7 @@
         <v>122</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>123</v>
@@ -2935,7 +2936,7 @@
         <v>127</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>128</v>
@@ -2944,7 +2945,7 @@
         <v>129</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>130</v>
@@ -2955,22 +2956,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="F5" s="10">
         <v>45603</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -2978,22 +2979,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete implementation of camera shop features
</commit_message>
<xml_diff>
--- a/camera-shop/src/main/resources/data.xlsx
+++ b/camera-shop/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\camera-shop\camera-shop\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050D0733-2656-4EA0-8A2A-AB2D26279F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27253079-90AA-45E3-B818-FF6611B641FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{90887BD4-D8A2-4FD5-939A-5967D6FE0B64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{90887BD4-D8A2-4FD5-939A-5967D6FE0B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Brand" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="252">
   <si>
     <t>id</t>
   </si>
@@ -284,52 +284,18 @@
     <t>White</t>
   </si>
   <si>
-    <t>Sony ZV-E1</t>
-  </si>
-  <si>
-    <t>399g</t>
-  </si>
-  <si>
-    <t>121 x 71.9 x 54.3 mm</t>
-  </si>
-  <si>
-    <t>1 x Pin NP-FZ100 Lithium-Ion (570 shots)</t>
-  </si>
-  <si>
-    <t>RawXAVC HS, UHD 4K, 1920 x 1080p, 3840 x 2160</t>
-  </si>
-  <si>
-    <t>Approx. 20.1 Megapixels</t>
-  </si>
-  <si>
-    <t>80 to 102,400 
-(Expandable: 80 to 409,600)</t>
-  </si>
-  <si>
-    <t>Digital, 5-axis</t>
-  </si>
-  <si>
     <t>Camera + Grip</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307772/camera/Sony%20ZV-E1/e284149f-d0c2-4d7c-b676-f43cb759fb30.png</t>
-  </si>
-  <si>
     <t>1, 2, 3, 5</t>
   </si>
   <si>
-    <t>1, 2, 3, 6</t>
-  </si>
-  <si>
     <t>Designed for vloggers, the Sony ZV-E10 camera combines a large sensor and the flexibility of a mirrorless camera to deliver high-quality images.</t>
   </si>
   <si>
     <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719304295/camera/Sony%20ZV-E10/1.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304305/camera/Sony%20ZV-E10/2.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304320/camera/Sony%20ZV-E10/3.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304338/camera/Sony%20ZV-E10/4.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304352/camera/Sony%20ZV-E10/5.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719304360/camera/Sony%20ZV-E10/6.png</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719306610/camera/Sony%20ZV-E1/3a57a97b-8981-4473-8daa-6c4370a03219.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719306638/camera/Sony%20ZV-E1/2263da14-968e-453b-978d-00536899ee27.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719306649/camera/Sony%20ZV-E1/2d65d2bd-799a-4e74-ba01-d76773e619a2.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307158/camera/Sony%20ZV-E1/9a6c35c6-3a67-42d0-a1f6-831ae43ef342.png</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719305162/camera/Sony%20ZV-E10/c5219028-5fad-4dde-b2ec-a5ba7bf36853.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305173/camera/Sony%20ZV-E10/1dd837f6-7392-4716-bef7-eb387644ed76.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305179/camera/Sony%20ZV-E10/9382b157-a86b-4186-b132-98da24e568a2.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305194/camera/Sony%20ZV-E10/e0bf3cd4-2dae-43ad-8dc8-2eb90aa61b68.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305205/camera/Sony%20ZV-E10/4856ef67-2b5d-48c0-b8cb-2331dbd8bf45.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305212/camera/Sony%20ZV-E10/0350603e-1717-4200-ba4c-94d3699eeee7.png</t>
   </si>
   <si>
@@ -337,12 +303,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719305543/camera/Sony%20ZV-E10/ae630dda-95ed-4be9-bc6b-2efe6e929fac.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719305555/camera/Sony%20ZV-E10/803943c0-2a6d-4e0e-842f-fce11f074f88.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305618/camera/Sony%20ZV-E10/394dd43e-7bf8-4633-8749-21c377a69dd0.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305568/camera/Sony%20ZV-E10/13192b7e-dea6-458c-b39d-4991927065e8.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305627/camera/Sony%20ZV-E10/8613dc9c-8ce2-4bf1-bac0-cd1eb7bd1e5d.png</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307624/camera/Sony%20ZV-E1/17a716f9-9b1a-4fb0-8fb7-0d1d6a59ce41.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307640/camera/Sony%20ZV-E1/8017131e-93cb-44a8-ba40-c83655f1388e.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307615/camera/Sony%20ZV-E1/fb085051-4096-4f9e-a6a9-1ce5adb4d040.png</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307710/camera/Sony%20ZV-E1/aaa0d6a1-c5df-4cab-9ccf-29396557b96a.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719307696/camera/Sony%20ZV-E1/99273871-d0a9-44d1-a4a3-2bdcddb254a7.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307715/camera/Sony%20ZV-E1/581b678f-d7da-4dae-acb5-6a3cc76a5f16.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307723/camera/Sony%20ZV-E1/0339be64-e64d-4584-8392-a8d602940b33.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307731/camera/Sony%20ZV-E1/fe0b854d-1f49-4ef3-a3cc-7ec9cbda9aa4.png</t>
   </si>
   <si>
     <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719812989/camera/category/selfie.jpg</t>
@@ -472,16 +432,10 @@
     <t>Actual: 26.1 Megapixel (6240 x 4160)</t>
   </si>
   <si>
-    <t>DCI 4K (4096 x 2160) ; Full HD (1920 x 1080)</t>
-  </si>
-  <si>
     <t>1 x NP-W235 Lithium-Ion, 7.2 VDC, 2200 mAh (600 shots)</t>
   </si>
   <si>
     <t>134.6 x 92.8 x 63.8 mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Sony ZV-E1 is a versatile camera that is well-suited for content creators. It is compact and lightweight, making it easy to carry around, and it features a full-frame sensor and powerful image processor that can capture high-quality images and videos. </t>
   </si>
   <si>
     <t>Auto, ISO 160 to 12800 
@@ -768,9 +722,6 @@
     <t>Up to 11 fps at 24.2MP for up to 116 Frames (JPEG) / 46 Frames (RAW)</t>
   </si>
   <si>
-    <t>Speed Priority Continuous Shooting: approx. 16fps, Continuous Shooting: approx. 3.5fps</t>
-  </si>
-  <si>
     <t>The Fujifilm X-T4 is a powerful mirrorless camera that combines a robust, weather-sealed body with professional features for both photo and video.</t>
   </si>
   <si>
@@ -780,10 +731,132 @@
     <t>Understanding how your sensor responds can open up creative options that aren't otherwise obvious. For instance, this high dynamic range scene was achieved using a single exposure, thanks to the camera's excellent noise characteristics.</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307531/camera/Sony%20ZV-E1/808593c8-c5ef-4fb4-a31c-506bc81b793e.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719307544/camera/Sony%20ZV-E1/f8bc95b0-d67d-4e21-90e1-9ed2d6db1e7a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307578/camera/Sony%20ZV-E1/a5d6be80-68f6-4d70-b4ec-c2aa84ab8919.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307602/camera/Sony%20ZV-E1/91e001c1-d281-4f95-bd6c-3d3c30370122.png</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721131052/camera/Leica%20Q2/a1614e9a-7c82-47ab-8538-0cf546cf162d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131058/camera/Leica%20Q2/c9c25964-dda5-4170-91ed-b77f819de908.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131065/camera/Leica%20Q2/d5522030-38b2-4a4f-b31b-477500938282.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131067/camera/Leica%20Q2/7bc53414-d61e-439a-9ada-d3f8e2dc0728.png</t>
+  </si>
+  <si>
+    <t>Sony ZV-1F</t>
+  </si>
+  <si>
+    <t>Specifically designed for vloggers and online content creators, the Sony ZV-1F Vlogging Camera is a “pocket-sized” camera boasting a large 1-inch sensor, a wide-angle ZEISS lens with a 20mm equivalent focal length, the new-generation BIONZ X image processor, support for UHD 4K30p video recording, unique 5x Slow Motion &amp; 60x Hyperlapse modes, a 3.0-inch flip-up touchscreen LCD, high-quality livestreaming, and many other outstanding features.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Auto, ISO 125 to 12800</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>Electronic shutter
+Up to 16 frames per second (JPEG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+20.1 Megapixel (5472 x 3648)</t>
+  </si>
+  <si>
+    <t>DCI 4K (4096 x 2160); Full HD (1920 x 1080)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1 x Pin NP-BX1 Lithium-Ion 1240 mAh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+229g</t>
+  </si>
+  <si>
+    <t>105.6 x 60 x 46.4 mm</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721889816/camera/Sony%20ZV-1F/32749466-9cb7-4040-a631-333c8f22b72c.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721889827/camera/Sony%20ZV-1F/233985d0-342a-4c5c-aaf0-b34e5d5ffa4b.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721889831/camera/Sony%20ZV-1F/f49673a2-65e1-46ba-9c67-ad0f36531d14.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721889844/camera/Sony%20ZV-1F/6d9bb8d9-0a67-47de-b8ff-5db7bd5d8bca.png</t>
+  </si>
+  <si>
+    <t>Nikon Z50</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>A compact and lightweight mirrorless camera designed for vlogging and travel with a wide range of features.</t>
+  </si>
+  <si>
+    <t>Auto, ISO 100 to 51200</t>
+  </si>
+  <si>
+    <t>Up to 11 fps</t>
+  </si>
+  <si>
+    <t>20.9 Megapixel</t>
+  </si>
+  <si>
+    <t>1 x EN-EL25 Lithium-Ion, 7.6 VDC, 1120 mAh (300 shots)</t>
+  </si>
+  <si>
+    <t>126.5 x 93.5 x 60 mm</t>
+  </si>
+  <si>
+    <t>4K UHD (3840 x 2160); Full HD (1920 x 1080)</t>
+  </si>
+  <si>
+    <t>395 g</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721890864/camera/Nikon%20Z50/0d1b6652-7fea-4f99-b91f-7d1dcaf925ca.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721890873/camera/Nikon%20Z50/9410d80c-4a3e-41a2-803d-d6dc1c8f869b.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721890880/camera/Nikon%20Z50/1103b277-5c5f-4608-83c2-7ba1bf7ac116.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721890883/camera/Nikon%20Z50/3389ab98-f3d3-4348-b5d1-2cbeb818d1de.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721890734/camera/Nikon%20Z50/6294f598-e459-4bab-8ed0-62970719c7ea.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721890747/camera/Nikon%20Z50/bd1f6ed8-cc5c-4d4a-aac0-808183a17a72.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721890759/camera/Nikon%20Z50/23b69410-8fa7-4800-a9fb-02b91424a55f.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721890754/camera/Nikon%20Z50/97ab6bfd-eac6-49dc-bedb-b48029d7edf3.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721890846/camera/Nikon%20Z50/bc3503dd-4e68-433f-bf70-5350cc16bc3e.png</t>
+  </si>
+  <si>
+    <t>Leica M11</t>
+  </si>
+  <si>
+    <t>1, 4, 5</t>
+  </si>
+  <si>
+    <t>The Leica M11 is a rangefinder camera that embodies the familiar design of the Leica M series. While its external design remains largely unchanged, the camera boasts significant internal upgrades, resulting in a unique user experience. It's a perfect fit for those who appreciate a classic and refined style.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Auto, ISO 64 to 50000</t>
+  </si>
+  <si>
+    <t>Up to 4.5 fps</t>
+  </si>
+  <si>
+    <t>60 Megapixel</t>
+  </si>
+  <si>
+    <t>Full HD (1920 x 1080)</t>
+  </si>
+  <si>
+    <t>1 x BP-SCL5 Lithium-Ion, 7.4 VDC, 1800 mAh (700 shots)</t>
+  </si>
+  <si>
+    <t>139 x 80 x 38.5 mm</t>
+  </si>
+  <si>
+    <t>530 g</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721891592/camera/Leica%20M11/8ef94943-f2c4-4029-bbf3-25f1fde63eab.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721891561/camera/Leica%20M11/b049d0d0-5089-4386-8834-cf2d706fd015.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721891604/camera/Leica%20M11/7506f5b4-2024-47c3-a181-e3708ca15c6c.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721891608/camera/Leica%20M11/f5cdeb18-54b5-46e7-a5a5-425a97529bef.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1721891507/camera/Leica%20M11/5b8049ac-191a-4810-9d66-6eed592f8d8c.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721891543/camera/Leica%20M11/20d7b1d9-22a9-4cd9-8b7b-4ad58d7780d9.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721891512/camera/Leica%20M11/e88940d3-1bc2-4553-a940-93ffa52a7547.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721891575/camera/Leica%20M11/27b7cd6b-b6e4-4072-81c2-1fb664314e67.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721891537/camera/Leica%20M11/ae8749b6-abb0-4fb5-965d-da9cfab25bfc.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721891585/camera/Leica%20M11/518e1d78-b5d7-4497-8e57-82506cd57fd5.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307544/camera/Sony%20ZV-1F/f8bc95b0-d67d-4e21-90e1-9ed2d6db1e7a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307531/camera/Sony%20ZV-1F/808593c8-c5ef-4fb4-a31c-506bc81b793e.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307578/camera/Sony%20ZV-1F/a5d6be80-68f6-4d70-b4ec-c2aa84ab8919.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307555/camera/Sony%20ZV-1F/dcde0034-6ee4-458b-bfd9-7f18e69e8896.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307602/camera/Sony%20ZV-1F/91e001c1-d281-4f95-bd6c-3d3c30370122.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307624/camera/Sony%20ZV-1F/17a716f9-9b1a-4fb0-8fb7-0d1d6a59ce41.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307615/camera/Sony%20ZV-1F/fb085051-4096-4f9e-a6a9-1ce5adb4d040.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307640/camera/Sony%20ZV-1F/8017131e-93cb-44a8-ba40-c83655f1388e.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307696/camera/Sony%20ZV-1F/99273871-d0a9-44d1-a4a3-2bdcddb254a7.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307710/camera/Sony%20ZV-1F/aaa0d6a1-c5df-4cab-9ccf-29396557b96a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307715/camera/Sony%20ZV-1F/581b678f-d7da-4dae-acb5-6a3cc76a5f16.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307723/camera/Sony%20ZV-1F/0339be64-e64d-4584-8392-a8d602940b33.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307731/camera/Sony%20ZV-1F/fe0b854d-1f49-4ef3-a3cc-7ec9cbda9aa4.png</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dwywbuukd/image/upload/v1719307772/camera/Sony%20ZV-1F/e284149f-d0c2-4d7c-b676-f43cb759fb30.png</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1276,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,7 +1312,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1256,7 +1329,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -1273,7 +1346,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -1290,7 +1363,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -1307,7 +1380,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -1333,7 +1406,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,7 +1443,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
         <v>43</v>
@@ -1387,7 +1460,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
@@ -1404,7 +1477,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
         <v>51</v>
@@ -1421,7 +1494,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
@@ -1438,7 +1511,7 @@
         <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
         <v>53</v>
@@ -1455,7 +1528,7 @@
         <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
@@ -1472,7 +1545,7 @@
         <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
         <v>55</v>
@@ -1500,7 +1573,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1583,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DE6A29-D1BE-4327-A15B-C071AAA1973B}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K3" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1688,19 +1761,19 @@
         <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="K2" t="s">
         <v>57</v>
@@ -1724,18 +1797,18 @@
         <v>1</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="173.4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>212</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1747,43 +1820,43 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>137</v>
+        <v>213</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>86</v>
+        <v>214</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" t="s">
-        <v>85</v>
+        <v>215</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="L3" t="s">
         <v>59</v>
       </c>
       <c r="M3" t="s">
-        <v>84</v>
-      </c>
-      <c r="N3" t="s">
-        <v>83</v>
-      </c>
-      <c r="O3" t="s">
-        <v>81</v>
-      </c>
-      <c r="P3" t="s">
-        <v>82</v>
+        <v>160</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>94</v>
+        <v>222</v>
       </c>
       <c r="S3">
         <v>1</v>
@@ -1794,7 +1867,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1806,43 +1879,43 @@
         <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="L4" t="s">
         <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>134</v>
+        <v>218</v>
       </c>
       <c r="N4" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="P4" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="Q4">
         <v>1</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="S4">
         <v>1</v>
@@ -1853,7 +1926,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -1865,43 +1938,43 @@
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="K5" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="L5" t="s">
         <v>59</v>
       </c>
       <c r="M5" t="s">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="N5" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="P5" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -1912,7 +1985,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -1924,43 +1997,43 @@
         <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="L6" t="s">
         <v>59</v>
       </c>
       <c r="M6" t="s">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="Q6">
         <v>1</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -1971,7 +2044,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -1983,43 +2056,43 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="K7" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="L7" t="s">
         <v>59</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>134</v>
+        <v>218</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="P7" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="Q7">
         <v>1</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="S7">
         <v>1</v>
@@ -2030,7 +2103,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -2042,43 +2115,43 @@
         <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="L8" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="M8" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="N8" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="O8" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="P8" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -2089,7 +2162,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -2101,45 +2174,163 @@
         <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="N9" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="O9" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="P9" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="43.8" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>224</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="H10" t="s">
+        <v>226</v>
+      </c>
+      <c r="I10" t="s">
+        <v>227</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="S9">
+      <c r="K10" t="s">
+        <v>228</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="M10" t="s">
+        <v>231</v>
+      </c>
+      <c r="N10" t="s">
+        <v>229</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="P10" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>233</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="115.8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>236</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H11" t="s">
+        <v>239</v>
+      </c>
+      <c r="I11" t="s">
+        <v>240</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="K11" t="s">
+        <v>241</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="M11" t="s">
+        <v>242</v>
+      </c>
+      <c r="N11" t="s">
+        <v>243</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>246</v>
+      </c>
+      <c r="S11">
         <v>1</v>
       </c>
     </row>
@@ -2151,15 +2342,18 @@
     <hyperlink ref="R7" r:id="rId3" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1721131052/camera/Leica%20Q2/a1614e9a-7c82-47ab-8538-0cf546cf162d.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131058/camera/Leica%20Q2/c9c25964-dda5-4170-91ed-b77f819de908.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131065/camera/Leica%20Q2/d5522030-38b2-4a4f-b31b-477500938282.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1721131067/camera/Leica%20Q2/7bc53414-d61e-439a-9ada-d3f8e2dc0728.png" xr:uid="{302D02AB-12FB-4CA3-BC27-F302994B1DF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F11" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D78C07-7927-4BB8-A0DC-CDDE00B048CF}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2170,7 +2364,7 @@
     <col min="6" max="6" width="21.77734375" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="10" max="10" width="64.88671875" customWidth="1"/>
     <col min="11" max="11" width="8.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2238,7 +2432,7 @@
         <v>950</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -2273,7 +2467,7 @@
         <v>1300</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -2308,7 +2502,7 @@
         <v>950</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -2328,7 +2522,7 @@
         <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G5">
         <v>7</v>
@@ -2340,7 +2534,7 @@
         <v>620</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -2372,7 +2566,7 @@
         <v>950</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>98</v>
+        <v>249</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -2392,7 +2586,7 @@
         <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -2404,7 +2598,7 @@
         <v>620</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>99</v>
+        <v>250</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -2424,7 +2618,7 @@
         <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G8">
         <v>8</v>
@@ -2436,7 +2630,7 @@
         <v>770</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>89</v>
+        <v>251</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -2456,7 +2650,7 @@
         <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="F9" t="s">
         <v>77</v>
@@ -2471,7 +2665,7 @@
         <v>1260</v>
       </c>
       <c r="J9" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -2488,10 +2682,10 @@
         <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="E10" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="F10" t="s">
         <v>77</v>
@@ -2506,7 +2700,7 @@
         <v>1380</v>
       </c>
       <c r="J10" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -2526,7 +2720,7 @@
         <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G11">
         <v>5</v>
@@ -2538,7 +2732,7 @@
         <v>1480</v>
       </c>
       <c r="J11" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -2558,7 +2752,7 @@
         <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2570,7 +2764,7 @@
         <v>3800</v>
       </c>
       <c r="J12" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -2590,7 +2784,7 @@
         <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -2602,7 +2796,7 @@
         <v>1500</v>
       </c>
       <c r="J13" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -2622,7 +2816,7 @@
         <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -2634,7 +2828,7 @@
         <v>2050</v>
       </c>
       <c r="J14" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -2663,7 +2857,7 @@
         <v>5100</v>
       </c>
       <c r="J15" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -2683,7 +2877,7 @@
         <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -2695,7 +2889,7 @@
         <v>500</v>
       </c>
       <c r="J16" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -2715,7 +2909,7 @@
         <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -2727,7 +2921,7 @@
         <v>550</v>
       </c>
       <c r="J17" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -2747,7 +2941,7 @@
         <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2759,7 +2953,7 @@
         <v>550</v>
       </c>
       <c r="J18" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2779,7 +2973,7 @@
         <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G19">
         <v>3</v>
@@ -2791,7 +2985,7 @@
         <v>2200</v>
       </c>
       <c r="J19" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -2811,7 +3005,7 @@
         <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -2823,9 +3017,73 @@
         <v>2900</v>
       </c>
       <c r="J20" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="K20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
+        <v>183</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>675</v>
+      </c>
+      <c r="J21" t="s">
+        <v>234</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>183</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+      <c r="I22">
+        <v>7500</v>
+      </c>
+      <c r="J22" t="s">
+        <v>247</v>
+      </c>
+      <c r="K22">
         <v>1</v>
       </c>
     </row>
@@ -2835,8 +3093,8 @@
     <hyperlink ref="J3" r:id="rId2" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1719305429/camera/Sony%20ZV-E10/971bf35e-c475-4d68-be23-c204f036c259.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305441/camera/Sony%20ZV-E10/9c89118e-4ea4-4f2f-afe5-0306cc2d707f.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305485/camera/Sony%20ZV-E10/c4d863b2-ad86-4a1f-bb8b-2ec667e0cd56.png" xr:uid="{AE5D3DA8-C194-4FB0-AB6F-2A7485BF6B0F}"/>
     <hyperlink ref="J4" r:id="rId3" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1719305543/camera/Sony%20ZV-E10/ae630dda-95ed-4be9-bc6b-2efe6e929fac.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719305555/camera/Sony%20ZV-E10/803943c0-2a6d-4e0e-842f-fce11f074f88.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305618/camera/Sony%20ZV-E10/394dd43e-7bf8-4633-8749-21c377a69dd0.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305568/camera/Sony%20ZV-E10/13192b7e-dea6-458c-b39d-4991927065e8.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719305627/camera/Sony%20ZV-E10/8613dc9c-8ce2-4bf1-bac0-cd1eb7bd1e5d.png" xr:uid="{DEB50EFF-2B63-4045-BCD4-3FB022C66E5F}"/>
     <hyperlink ref="J5" r:id="rId4" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1719307531/camera/Sony%20ZV-E1/808593c8-c5ef-4fb4-a31c-506bc81b793e.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719307544/camera/Sony%20ZV-E1/f8bc95b0-d67d-4e21-90e1-9ed2d6db1e7a.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307578/camera/Sony%20ZV-E1/a5d6be80-68f6-4d70-b4ec-c2aa84ab8919.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307578/camera/Sony%20ZV-E1/a5d6be80-68f6-4d70-b4ec-c2aa84ab8919.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307602/camera/Sony%20ZV-E1/91e001c1-d281-4f95-bd6c-3d3c30370122.png" xr:uid="{D80AABE7-79D3-4052-BACC-A064D057CF51}"/>
-    <hyperlink ref="J6" r:id="rId5" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1719307624/camera/Sony%20ZV-E1/17a716f9-9b1a-4fb0-8fb7-0d1d6a59ce41.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307640/camera/Sony%20ZV-E1/8017131e-93cb-44a8-ba40-c83655f1388e.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307615/camera/Sony%20ZV-E1/fb085051-4096-4f9e-a6a9-1ce5adb4d040.png" xr:uid="{62E208BE-B0D3-46E7-B824-E732B9D2E3E1}"/>
-    <hyperlink ref="J7" r:id="rId6" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1719307710/camera/Sony%20ZV-E1/aaa0d6a1-c5df-4cab-9ccf-29396557b96a.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719307696/camera/Sony%20ZV-E1/99273871-d0a9-44d1-a4a3-2bdcddb254a7.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307715/camera/Sony%20ZV-E1/581b678f-d7da-4dae-acb5-6a3cc76a5f16.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307723/camera/Sony%20ZV-E1/0339be64-e64d-4584-8392-a8d602940b33.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307731/camera/Sony%20ZV-E1/fe0b854d-1f49-4ef3-a3cc-7ec9cbda9aa4.png" xr:uid="{B8309DB8-B6F2-42CE-84A0-14DF9F80CCAE}"/>
+    <hyperlink ref="J7" r:id="rId5" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1719307710/camera/Sony%20ZV-E1/aaa0d6a1-c5df-4cab-9ccf-29396557b96a.png, https://res.cloudinary.com/dwywbuukd/image/upload/v1719307696/camera/Sony%20ZV-E1/99273871-d0a9-44d1-a4a3-2bdcddb254a7.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307715/camera/Sony%20ZV-E1/581b678f-d7da-4dae-acb5-6a3cc76a5f16.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307723/camera/Sony%20ZV-E1/0339be64-e64d-4584-8392-a8d602940b33.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307731/camera/Sony%20ZV-E1/fe0b854d-1f49-4ef3-a3cc-7ec9cbda9aa4.png" xr:uid="{B8309DB8-B6F2-42CE-84A0-14DF9F80CCAE}"/>
+    <hyperlink ref="J6" r:id="rId6" display="https://res.cloudinary.com/dwywbuukd/image/upload/v1719307624/camera/Sony%20ZV-1F/17a716f9-9b1a-4fb0-8fb7-0d1d6a59ce41.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307615/camera/Sony%20ZV-1F/fb085051-4096-4f9e-a6a9-1ce5adb4d040.png,https://res.cloudinary.com/dwywbuukd/image/upload/v1719307640/camera/Sony%20ZV-1F/8017131e-93cb-44a8-ba40-c83655f1388e.png" xr:uid="{62E208BE-B0D3-46E7-B824-E732B9D2E3E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2864,19 +3122,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>4</v>
@@ -2887,22 +3145,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F2" s="5">
         <v>45389</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -2910,22 +3168,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -2933,22 +3191,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -2956,22 +3214,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="F5" s="10">
         <v>45603</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -2979,22 +3237,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>